<commit_message>
Contining improvements to US national table and trying to plot
</commit_message>
<xml_diff>
--- a/Sources/12s0306-tot_in_thousands_ofcrimetype1980-2009.xlsx
+++ b/Sources/12s0306-tot_in_thousands_ofcrimetype1980-2009.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Year</t>
   </si>
@@ -102,6 +105,39 @@
   </si>
   <si>
     <t>Murder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1989</t>
   </si>
 </sst>
 </file>
@@ -143,8 +179,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -453,15 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,510 +548,1010 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1960</v>
+      </c>
+      <c r="D2">
+        <v>9.11</v>
+      </c>
+      <c r="E2">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="H2">
+        <v>17190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1961</v>
+      </c>
+      <c r="D3">
+        <v>8.74</v>
+      </c>
+      <c r="E3">
+        <v>17.22</v>
+      </c>
+      <c r="H3">
+        <v>17220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1962</v>
+      </c>
+      <c r="D4">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="E4">
+        <v>17.55</v>
+      </c>
+      <c r="H4">
+        <v>17550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1963</v>
+      </c>
+      <c r="D5">
+        <v>8.64</v>
+      </c>
+      <c r="E5">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="H5">
+        <v>17650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1964</v>
+      </c>
+      <c r="D6">
+        <v>9.36</v>
+      </c>
+      <c r="E6">
+        <v>21.42</v>
+      </c>
+      <c r="H6">
+        <v>21420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1965</v>
+      </c>
+      <c r="D7">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="E7">
+        <v>23.41</v>
+      </c>
+      <c r="H7">
+        <v>23410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1966</v>
+      </c>
+      <c r="D8">
+        <v>11.04</v>
+      </c>
+      <c r="E8">
+        <v>25.82</v>
+      </c>
+      <c r="H8">
+        <v>25820</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1967</v>
+      </c>
+      <c r="D9">
+        <v>12.24</v>
+      </c>
+      <c r="E9">
+        <v>27.62</v>
+      </c>
+      <c r="H9">
+        <v>27620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1968</v>
+      </c>
+      <c r="D10">
+        <v>13.8</v>
+      </c>
+      <c r="E10">
+        <v>31.67</v>
+      </c>
+      <c r="H10">
+        <v>31670</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1969</v>
+      </c>
+      <c r="D11">
+        <v>14.76</v>
+      </c>
+      <c r="E11">
+        <v>37.17</v>
+      </c>
+      <c r="H11">
+        <v>37170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1970</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>37.99</v>
+      </c>
+      <c r="H12">
+        <v>37990</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1971</v>
+      </c>
+      <c r="D13">
+        <v>17.78</v>
+      </c>
+      <c r="E13">
+        <v>42.26</v>
+      </c>
+      <c r="H13">
+        <v>42260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1972</v>
+      </c>
+      <c r="D14">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="E14">
+        <v>46.85</v>
+      </c>
+      <c r="H14">
+        <v>46850</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1973</v>
+      </c>
+      <c r="D15">
+        <v>19.64</v>
+      </c>
+      <c r="E15">
+        <v>51.4</v>
+      </c>
+      <c r="H15">
+        <v>51400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1974</v>
+      </c>
+      <c r="D16">
+        <v>20.71</v>
+      </c>
+      <c r="E16">
+        <v>55.4</v>
+      </c>
+      <c r="H16">
+        <v>55400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1975</v>
+      </c>
+      <c r="D17">
+        <v>20.51</v>
+      </c>
+      <c r="E17">
+        <v>56.09</v>
+      </c>
+      <c r="H17">
+        <v>56090</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1976</v>
+      </c>
+      <c r="D18">
+        <v>18.78</v>
+      </c>
+      <c r="E18">
+        <v>57.08</v>
+      </c>
+      <c r="H18">
+        <v>57080</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1977</v>
+      </c>
+      <c r="D19">
+        <v>19.12</v>
+      </c>
+      <c r="E19">
+        <v>63.5</v>
+      </c>
+      <c r="H19">
+        <v>63500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1978</v>
+      </c>
+      <c r="D20">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="E20">
+        <v>67.61</v>
+      </c>
+      <c r="H20">
+        <v>67610</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1979</v>
+      </c>
+      <c r="D21">
+        <v>21.46</v>
+      </c>
+      <c r="E21">
+        <v>76.39</v>
+      </c>
+      <c r="H21">
+        <v>76390</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B22">
         <v>13408.3</v>
       </c>
-      <c r="C2">
+      <c r="C22">
         <v>1344.52</v>
       </c>
-      <c r="D2">
+      <c r="D22">
         <v>23.04</v>
       </c>
-      <c r="E2">
+      <c r="E22">
         <v>82.99</v>
       </c>
-      <c r="F2">
+      <c r="F22">
         <v>565.84</v>
       </c>
-      <c r="G2">
+      <c r="G22">
         <v>672.65</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H22">
+        <v>82990</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23">
+        <v>22.52</v>
+      </c>
+      <c r="E23">
+        <v>82.5</v>
+      </c>
+      <c r="H23">
+        <v>82500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24">
+        <v>21.01</v>
+      </c>
+      <c r="E24">
+        <v>78.77</v>
+      </c>
+      <c r="H24">
+        <v>78770</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>19.308</v>
+      </c>
+      <c r="E25">
+        <v>78.918000000000006</v>
+      </c>
+      <c r="H25">
+        <v>78918</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26">
+        <v>18.692</v>
+      </c>
+      <c r="E26">
+        <v>84.233000000000004</v>
+      </c>
+      <c r="H26">
+        <v>84233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B27">
         <v>12430.357</v>
       </c>
-      <c r="C3">
+      <c r="C27">
         <v>1327.7670000000001</v>
       </c>
-      <c r="D3">
+      <c r="D27">
         <v>18.975999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E27">
         <v>87.671000000000006</v>
       </c>
-      <c r="F3">
+      <c r="F27">
         <v>497.87400000000002</v>
       </c>
-      <c r="G3">
+      <c r="G27">
         <v>723.24599999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H27">
+        <v>87671</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>20.613</v>
+      </c>
+      <c r="E28">
+        <v>91.459000000000003</v>
+      </c>
+      <c r="H28">
+        <v>91459</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29">
+        <v>20.096</v>
+      </c>
+      <c r="E29">
+        <v>91.111000000000004</v>
+      </c>
+      <c r="H29">
+        <v>91111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>20.675000000000001</v>
+      </c>
+      <c r="E30">
+        <v>92.486000000000004</v>
+      </c>
+      <c r="H30">
+        <v>92486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>21.5</v>
+      </c>
+      <c r="E31">
+        <v>94.504000000000005</v>
+      </c>
+      <c r="H31">
+        <v>94504</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B32">
         <v>14475.6</v>
       </c>
-      <c r="C4">
+      <c r="C32">
         <v>1820.127</v>
       </c>
-      <c r="D4">
+      <c r="D32">
         <v>23.437999999999999</v>
       </c>
-      <c r="E4">
+      <c r="E32">
         <v>102.55500000000001</v>
       </c>
-      <c r="F4">
+      <c r="F32">
         <v>639.27099999999996</v>
       </c>
-      <c r="G4">
+      <c r="G32">
         <v>1054.8630000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="H32">
+        <v>102555</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>1991</v>
       </c>
-      <c r="B5">
+      <c r="B33">
         <v>14872.9</v>
       </c>
-      <c r="C5">
+      <c r="C33">
         <v>1911.7670000000001</v>
       </c>
-      <c r="D5">
+      <c r="D33">
         <v>24.702999999999999</v>
       </c>
-      <c r="E5">
+      <c r="E33">
         <v>106.593</v>
       </c>
-      <c r="F5">
+      <c r="F33">
         <v>687.73199999999997</v>
       </c>
-      <c r="G5">
+      <c r="G33">
         <v>1092.739</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="H33">
+        <v>106593</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>1992</v>
       </c>
-      <c r="B6">
+      <c r="B34">
         <v>14438.191000000001</v>
       </c>
-      <c r="C6">
+      <c r="C34">
         <v>1932.2739999999999</v>
       </c>
-      <c r="D6">
+      <c r="D34">
         <v>23.76</v>
       </c>
-      <c r="E6">
+      <c r="E34">
         <v>109.062</v>
       </c>
-      <c r="F6">
+      <c r="F34">
         <v>672.47799999999995</v>
       </c>
-      <c r="G6">
+      <c r="G34">
         <v>1126.9739999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H34">
+        <v>109062</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B35">
         <v>14144.8</v>
       </c>
-      <c r="C7">
+      <c r="C35">
         <v>1926.0170000000001</v>
       </c>
-      <c r="D7">
+      <c r="D35">
         <v>24.526</v>
       </c>
-      <c r="E7">
+      <c r="E35">
         <v>106.014</v>
       </c>
-      <c r="F7">
+      <c r="F35">
         <v>659.87</v>
       </c>
-      <c r="G7">
+      <c r="G35">
         <v>1135.607</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="H35">
+        <v>106014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B36">
         <v>13990</v>
       </c>
-      <c r="C8">
+      <c r="C36">
         <v>1857.67</v>
       </c>
-      <c r="D8">
+      <c r="D36">
         <v>23.326000000000001</v>
       </c>
-      <c r="E8">
+      <c r="E36">
         <v>102.21599999999999</v>
       </c>
-      <c r="F8">
+      <c r="F36">
         <v>618.94899999999996</v>
       </c>
-      <c r="G8">
+      <c r="G36">
         <v>1113.1790000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="H36">
+        <v>102216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B37">
         <v>13863</v>
       </c>
-      <c r="C9">
+      <c r="C37">
         <v>1798.7919999999999</v>
       </c>
-      <c r="D9">
+      <c r="D37">
         <v>21.606000000000002</v>
       </c>
-      <c r="E9">
+      <c r="E37">
         <v>97.47</v>
       </c>
-      <c r="F9">
+      <c r="F37">
         <v>580.50900000000001</v>
       </c>
-      <c r="G9">
+      <c r="G37">
         <v>1099.2070000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="H37">
+        <v>97470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B38">
         <v>13493.9</v>
       </c>
-      <c r="C10">
+      <c r="C38">
         <v>1688.54</v>
       </c>
-      <c r="D10">
+      <c r="D38">
         <v>19.645</v>
       </c>
-      <c r="E10">
+      <c r="E38">
         <v>96.251999999999995</v>
       </c>
-      <c r="F10">
+      <c r="F38">
         <v>535.59400000000005</v>
       </c>
-      <c r="G10">
+      <c r="G38">
         <v>1037.049</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="H38">
+        <v>96252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B39">
         <v>13194.571</v>
       </c>
-      <c r="C11">
+      <c r="C39">
         <v>1636.096</v>
       </c>
-      <c r="D11">
+      <c r="D39">
         <v>18.207999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E39">
         <v>96.153000000000006</v>
       </c>
-      <c r="F11">
+      <c r="F39">
         <v>498.53399999999999</v>
       </c>
-      <c r="G11">
+      <c r="G39">
         <v>1023.201</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="H39">
+        <v>96153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B40">
         <v>12485.7</v>
       </c>
-      <c r="C12">
+      <c r="C40">
         <v>1533.8869999999999</v>
       </c>
-      <c r="D12">
+      <c r="D40">
         <v>16.974</v>
       </c>
-      <c r="E12">
+      <c r="E40">
         <v>93.144000000000005</v>
       </c>
-      <c r="F12">
+      <c r="F40">
         <v>447.18599999999998</v>
       </c>
-      <c r="G12">
+      <c r="G40">
         <v>976.58299999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="H40">
+        <v>93144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
+      <c r="B41">
         <v>11634.378000000001</v>
       </c>
-      <c r="C13">
+      <c r="C41">
         <v>1426.0440000000001</v>
       </c>
-      <c r="D13">
+      <c r="D41">
         <v>15.522</v>
       </c>
-      <c r="E13">
+      <c r="E41">
         <v>89.411000000000001</v>
       </c>
-      <c r="F13">
+      <c r="F41">
         <v>409.37099999999998</v>
       </c>
-      <c r="G13">
+      <c r="G41">
         <v>911.74</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="H41">
+        <v>89411</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
+      <c r="B42">
         <v>11608.07</v>
       </c>
-      <c r="C14">
+      <c r="C42">
         <v>1425.4859999999999</v>
       </c>
-      <c r="D14">
+      <c r="D42">
         <v>15.586</v>
       </c>
-      <c r="E14">
+      <c r="E42">
         <v>90.177999999999997</v>
       </c>
-      <c r="F14">
+      <c r="F42">
         <v>408.01600000000002</v>
       </c>
-      <c r="G14">
+      <c r="G42">
         <v>911.70600000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="H42">
+        <v>90178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>2001</v>
       </c>
-      <c r="B15">
+      <c r="B43">
         <v>11876.669</v>
       </c>
-      <c r="C15">
+      <c r="C43">
         <v>1439.48</v>
       </c>
-      <c r="D15">
+      <c r="D43">
         <v>16.036999999999999</v>
       </c>
-      <c r="E15">
+      <c r="E43">
         <v>90.863</v>
       </c>
-      <c r="F15">
+      <c r="F43">
         <v>423.55700000000002</v>
       </c>
-      <c r="G15">
+      <c r="G43">
         <v>909.02300000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H43">
+        <v>90863</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B44">
         <v>11878.954</v>
       </c>
-      <c r="C16">
+      <c r="C44">
         <v>1423.6769999999999</v>
       </c>
-      <c r="D16">
+      <c r="D44">
         <v>16.228999999999999</v>
       </c>
-      <c r="E16">
+      <c r="E44">
         <v>95.234999999999999</v>
       </c>
-      <c r="F16">
+      <c r="F44">
         <v>420.80599999999998</v>
       </c>
-      <c r="G16">
+      <c r="G44">
         <v>891.40700000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H44">
+        <v>95235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B45">
         <v>11826.537999999999</v>
       </c>
-      <c r="C17">
+      <c r="C45">
         <v>1383.6759999999999</v>
       </c>
-      <c r="D17">
+      <c r="D45">
         <v>16.527999999999999</v>
       </c>
-      <c r="E17">
+      <c r="E45">
         <v>93.882999999999996</v>
       </c>
-      <c r="F17">
+      <c r="F45">
         <v>414.23500000000001</v>
       </c>
-      <c r="G17">
+      <c r="G45">
         <v>859.03</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H45">
+        <v>93883</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
+      <c r="B46">
         <v>11679.474</v>
       </c>
-      <c r="C18">
+      <c r="C46">
         <v>1360.088</v>
       </c>
-      <c r="D18">
+      <c r="D46">
         <v>16.148</v>
       </c>
-      <c r="E18">
+      <c r="E46">
         <v>95.088999999999999</v>
       </c>
-      <c r="F18">
+      <c r="F46">
         <v>401.47</v>
       </c>
-      <c r="G18">
+      <c r="G46">
         <v>847.38099999999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="H46">
+        <v>95089</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
+      <c r="B47">
         <v>11565.319</v>
       </c>
-      <c r="C19">
+      <c r="C47">
         <v>1390.7449999999999</v>
       </c>
-      <c r="D19">
+      <c r="D47">
         <v>16.739999999999998</v>
       </c>
-      <c r="E19">
+      <c r="E47">
         <v>94.346999999999994</v>
       </c>
-      <c r="F19">
+      <c r="F47">
         <v>417.43799999999999</v>
       </c>
-      <c r="G19">
+      <c r="G47">
         <v>862.22</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="H47">
+        <v>94347</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B20">
+      <c r="B48">
         <v>11467.310000000001</v>
       </c>
-      <c r="C20">
+      <c r="C48">
         <v>1435.951</v>
       </c>
-      <c r="D20">
-        <v>17.318000000000001</v>
-      </c>
-      <c r="E20">
-        <v>94.781999999999996</v>
-      </c>
-      <c r="F20">
+      <c r="D48">
+        <v>17.309000000000001</v>
+      </c>
+      <c r="E48">
+        <v>94.471999999999994</v>
+      </c>
+      <c r="F48">
         <v>449.803</v>
       </c>
-      <c r="G20">
+      <c r="G48">
         <v>874.048</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="H48">
+        <v>94472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B21">
+      <c r="B49">
         <v>11294.805</v>
       </c>
-      <c r="C21">
+      <c r="C49">
         <v>1421.99</v>
       </c>
-      <c r="D21">
-        <v>17.157</v>
-      </c>
-      <c r="E21">
-        <v>91.873999999999995</v>
-      </c>
-      <c r="F21">
+      <c r="D49">
+        <v>17.128</v>
+      </c>
+      <c r="E49">
+        <v>92.16</v>
+      </c>
+      <c r="F49">
         <v>447.15499999999997</v>
       </c>
-      <c r="G21">
+      <c r="G49">
         <v>865.80399999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="H49">
+        <v>92160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="B22">
+      <c r="B50">
         <v>11167.778</v>
       </c>
-      <c r="C22">
+      <c r="C50">
         <v>1392.6289999999999</v>
       </c>
-      <c r="D22">
-        <v>16.442</v>
-      </c>
-      <c r="E22">
-        <v>90.478999999999999</v>
-      </c>
-      <c r="F22">
+      <c r="D50">
+        <v>16.465</v>
+      </c>
+      <c r="E50">
+        <v>90.75</v>
+      </c>
+      <c r="F50">
         <v>443.57400000000001</v>
       </c>
-      <c r="G22">
+      <c r="G50">
         <v>842.13400000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H50">
+        <v>90750</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B23">
+      <c r="B51">
         <v>10639.369000000001</v>
       </c>
-      <c r="C23">
+      <c r="C51">
         <v>1318.3979999999999</v>
       </c>
-      <c r="D23">
-        <v>15.241</v>
-      </c>
-      <c r="E23">
-        <v>88.096999999999994</v>
-      </c>
-      <c r="F23">
+      <c r="D51">
+        <v>15.398999999999999</v>
+      </c>
+      <c r="E51">
+        <v>89.241</v>
+      </c>
+      <c r="F51">
         <v>408.21699999999998</v>
       </c>
-      <c r="G23">
+      <c r="G51">
         <v>806.84299999999996</v>
+      </c>
+      <c r="H51">
+        <v>89241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52">
+        <v>14.722</v>
+      </c>
+      <c r="E52">
+        <v>85.593000000000004</v>
+      </c>
+      <c r="H52">
+        <v>85593</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53">
+        <v>14.661</v>
+      </c>
+      <c r="E53">
+        <v>84.174999999999997</v>
+      </c>
+      <c r="H53">
+        <v>84175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54">
+        <v>14.827</v>
+      </c>
+      <c r="E54">
+        <v>84.376000000000005</v>
+      </c>
+      <c r="H54">
+        <v>84376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>